<commit_message>
minor change. One of the recording sites was mislabeled.
</commit_message>
<xml_diff>
--- a/Mouse_workbooks/CH_160107_A.xlsx
+++ b/Mouse_workbooks/CH_160107_A.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glickfeld_lab\Documents\docubase\Mouse_workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charliehass/LabStuff/DocuBase/Mouse_workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="0" windowWidth="16725" windowHeight="17100" tabRatio="738" activeTab="3"/>
+    <workbookView xWindow="4080" yWindow="460" windowWidth="16720" windowHeight="17100" tabRatio="738" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -850,6 +850,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -859,15 +868,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -959,6 +959,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -969,18 +981,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1335,14 +1335,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="38.1" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="38" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="62.375" style="27" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="62.33203125" style="27" customWidth="1"/>
     <col min="3" max="16384" width="18.5" style="9" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="38.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="38" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>20</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>42339</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
@@ -1382,19 +1382,19 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="147.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="148" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="32"/>
     </row>
-    <row r="7" spans="1:2" ht="38.1" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="38" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:2" ht="38" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:2" ht="38" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:2" ht="38" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:2" ht="38" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:2" ht="38" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:2" ht="38" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15"/>
     </row>
   </sheetData>
@@ -1413,21 +1413,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19:I19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.125" style="35" customWidth="1"/>
-    <col min="6" max="6" width="7.125" style="21" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" style="35" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" style="21" customWidth="1"/>
     <col min="7" max="7" width="34.5" style="21" customWidth="1"/>
-    <col min="8" max="8" width="8.375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="1" customWidth="1"/>
     <col min="10" max="16384" width="15" style="1" hidden="1"/>
   </cols>
   <sheetData>
@@ -1453,13 +1453,13 @@
         <v>8</v>
       </c>
       <c r="B2" s="55"/>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
       <c r="H2" s="26" t="s">
         <v>30</v>
       </c>
@@ -1475,10 +1475,10 @@
       <c r="C3" s="45">
         <v>34</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
       <c r="H3" s="46"/>
       <c r="I3" s="47"/>
     </row>
@@ -1497,7 +1497,7 @@
       <c r="H4" s="50"/>
       <c r="I4" s="51"/>
     </row>
-    <row r="5" spans="1:9" ht="26.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="44"/>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
@@ -1527,11 +1527,11 @@
       <c r="F6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="42"/>
-      <c r="I6" s="43"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="40"/>
     </row>
     <row r="7" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -1552,11 +1552,11 @@
       <c r="F7" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="39"/>
-      <c r="I7" s="40"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="43"/>
     </row>
     <row r="8" spans="1:9" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -1577,11 +1577,11 @@
       <c r="F8" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="39"/>
-      <c r="I8" s="40"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="43"/>
     </row>
     <row r="9" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -1600,11 +1600,11 @@
       <c r="F9" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="39"/>
-      <c r="I9" s="40"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="43"/>
     </row>
     <row r="10" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -1613,9 +1613,9 @@
       <c r="D10" s="5"/>
       <c r="E10" s="36"/>
       <c r="F10" s="23"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="40"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="43"/>
     </row>
     <row r="11" spans="1:9" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -1636,11 +1636,11 @@
       <c r="F11" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="38" t="s">
+      <c r="G11" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="39"/>
-      <c r="I11" s="40"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="43"/>
     </row>
     <row r="12" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -1661,13 +1661,13 @@
       <c r="F12" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="39"/>
-      <c r="I12" s="40"/>
-    </row>
-    <row r="13" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="42"/>
+      <c r="I12" s="43"/>
+    </row>
+    <row r="13" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>2</v>
       </c>
@@ -1684,26 +1684,26 @@
       <c r="F13" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="39"/>
-      <c r="I13" s="40"/>
-    </row>
-    <row r="14" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="42"/>
+      <c r="I13" s="43"/>
+    </row>
+    <row r="14" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
       <c r="E14" s="36"/>
       <c r="F14" s="23"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="40"/>
-    </row>
-    <row r="15" spans="1:9" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="41"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="43"/>
+    </row>
+    <row r="15" spans="1:9" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>54</v>
@@ -1720,15 +1720,15 @@
       <c r="F15" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="39"/>
-      <c r="I15" s="40"/>
-    </row>
-    <row r="16" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="42"/>
+      <c r="I15" s="43"/>
+    </row>
+    <row r="16" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>55</v>
@@ -1745,15 +1745,15 @@
       <c r="F16" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="38" t="s">
+      <c r="G16" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="39"/>
-      <c r="I16" s="40"/>
-    </row>
-    <row r="17" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="42"/>
+      <c r="I16" s="43"/>
+    </row>
+    <row r="17" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
@@ -1768,928 +1768,1018 @@
       <c r="F17" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="38" t="s">
+      <c r="G17" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="39"/>
-      <c r="I17" s="40"/>
-    </row>
-    <row r="18" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="42"/>
+      <c r="I17" s="43"/>
+    </row>
+    <row r="18" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
       <c r="E18" s="36"/>
       <c r="F18" s="23"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="40"/>
-    </row>
-    <row r="19" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="41"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="43"/>
+    </row>
+    <row r="19" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
       <c r="E19" s="36"/>
       <c r="F19" s="23"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="40"/>
-    </row>
-    <row r="20" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="41"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="43"/>
+    </row>
+    <row r="20" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="5"/>
       <c r="E20" s="36"/>
       <c r="F20" s="23"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="40"/>
-    </row>
-    <row r="21" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="41"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="43"/>
+    </row>
+    <row r="21" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="5"/>
       <c r="E21" s="36"/>
       <c r="F21" s="23"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="40"/>
-    </row>
-    <row r="22" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="41"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="43"/>
+    </row>
+    <row r="22" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
       <c r="E22" s="36"/>
       <c r="F22" s="23"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="40"/>
-    </row>
-    <row r="23" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="41"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="43"/>
+    </row>
+    <row r="23" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="5"/>
       <c r="E23" s="36"/>
       <c r="F23" s="23"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="40"/>
-    </row>
-    <row r="24" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="41"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="43"/>
+    </row>
+    <row r="24" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="5"/>
       <c r="E24" s="36"/>
       <c r="F24" s="23"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="40"/>
-    </row>
-    <row r="25" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G24" s="41"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="43"/>
+    </row>
+    <row r="25" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="5"/>
       <c r="E25" s="36"/>
       <c r="F25" s="23"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="40"/>
-    </row>
-    <row r="26" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="41"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="43"/>
+    </row>
+    <row r="26" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="5"/>
       <c r="E26" s="36"/>
       <c r="F26" s="23"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="40"/>
-    </row>
-    <row r="27" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="41"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="43"/>
+    </row>
+    <row r="27" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="5"/>
       <c r="E27" s="36"/>
       <c r="F27" s="23"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="40"/>
-    </row>
-    <row r="28" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G27" s="41"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="43"/>
+    </row>
+    <row r="28" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="5"/>
       <c r="E28" s="36"/>
       <c r="F28" s="23"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="40"/>
-    </row>
-    <row r="29" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="41"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="43"/>
+    </row>
+    <row r="29" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="5"/>
       <c r="E29" s="36"/>
       <c r="F29" s="23"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="40"/>
-    </row>
-    <row r="30" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="41"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="43"/>
+    </row>
+    <row r="30" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="5"/>
       <c r="E30" s="36"/>
       <c r="F30" s="23"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="40"/>
-    </row>
-    <row r="31" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G30" s="41"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="43"/>
+    </row>
+    <row r="31" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="5"/>
       <c r="E31" s="36"/>
       <c r="F31" s="23"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="40"/>
-    </row>
-    <row r="32" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G31" s="41"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="43"/>
+    </row>
+    <row r="32" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="5"/>
       <c r="E32" s="36"/>
       <c r="F32" s="23"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="40"/>
-    </row>
-    <row r="33" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G32" s="41"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="43"/>
+    </row>
+    <row r="33" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="5"/>
       <c r="E33" s="36"/>
       <c r="F33" s="23"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="40"/>
-    </row>
-    <row r="34" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G33" s="41"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="43"/>
+    </row>
+    <row r="34" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="5"/>
       <c r="E34" s="36"/>
       <c r="F34" s="23"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="40"/>
-    </row>
-    <row r="35" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="41"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="43"/>
+    </row>
+    <row r="35" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="5"/>
       <c r="E35" s="36"/>
       <c r="F35" s="23"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="40"/>
-    </row>
-    <row r="36" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G35" s="41"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="43"/>
+    </row>
+    <row r="36" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="5"/>
       <c r="E36" s="36"/>
       <c r="F36" s="23"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="39"/>
-      <c r="I36" s="40"/>
-    </row>
-    <row r="37" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G36" s="41"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="43"/>
+    </row>
+    <row r="37" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="5"/>
       <c r="E37" s="36"/>
       <c r="F37" s="23"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="40"/>
-    </row>
-    <row r="38" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G37" s="41"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="43"/>
+    </row>
+    <row r="38" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="5"/>
       <c r="E38" s="36"/>
       <c r="F38" s="23"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="40"/>
-    </row>
-    <row r="39" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G38" s="41"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="43"/>
+    </row>
+    <row r="39" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="5"/>
       <c r="E39" s="36"/>
       <c r="F39" s="23"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="40"/>
-    </row>
-    <row r="40" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G39" s="41"/>
+      <c r="H39" s="42"/>
+      <c r="I39" s="43"/>
+    </row>
+    <row r="40" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="5"/>
       <c r="E40" s="36"/>
       <c r="F40" s="23"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="40"/>
-    </row>
-    <row r="41" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G40" s="41"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="43"/>
+    </row>
+    <row r="41" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="5"/>
       <c r="E41" s="36"/>
       <c r="F41" s="23"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="40"/>
-    </row>
-    <row r="42" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G41" s="41"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="43"/>
+    </row>
+    <row r="42" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="5"/>
       <c r="E42" s="36"/>
       <c r="F42" s="23"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="40"/>
-    </row>
-    <row r="43" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G42" s="41"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="43"/>
+    </row>
+    <row r="43" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="5"/>
       <c r="E43" s="36"/>
       <c r="F43" s="23"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="40"/>
-    </row>
-    <row r="44" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G43" s="41"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="43"/>
+    </row>
+    <row r="44" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="5"/>
       <c r="E44" s="36"/>
       <c r="F44" s="23"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="40"/>
-    </row>
-    <row r="45" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G44" s="41"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="43"/>
+    </row>
+    <row r="45" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="5"/>
       <c r="E45" s="36"/>
       <c r="F45" s="23"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="40"/>
-    </row>
-    <row r="46" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G45" s="41"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="43"/>
+    </row>
+    <row r="46" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="5"/>
       <c r="E46" s="36"/>
       <c r="F46" s="23"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="39"/>
-      <c r="I46" s="40"/>
-    </row>
-    <row r="47" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G46" s="41"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="43"/>
+    </row>
+    <row r="47" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="5"/>
       <c r="E47" s="36"/>
       <c r="F47" s="23"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="39"/>
-      <c r="I47" s="40"/>
-    </row>
-    <row r="48" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G47" s="41"/>
+      <c r="H47" s="42"/>
+      <c r="I47" s="43"/>
+    </row>
+    <row r="48" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="5"/>
       <c r="E48" s="36"/>
       <c r="F48" s="23"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="39"/>
-      <c r="I48" s="40"/>
-    </row>
-    <row r="49" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G48" s="41"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="43"/>
+    </row>
+    <row r="49" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="5"/>
       <c r="E49" s="36"/>
       <c r="F49" s="23"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="39"/>
-      <c r="I49" s="40"/>
-    </row>
-    <row r="50" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G49" s="41"/>
+      <c r="H49" s="42"/>
+      <c r="I49" s="43"/>
+    </row>
+    <row r="50" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="5"/>
       <c r="E50" s="36"/>
       <c r="F50" s="23"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="39"/>
-      <c r="I50" s="40"/>
-    </row>
-    <row r="51" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G50" s="41"/>
+      <c r="H50" s="42"/>
+      <c r="I50" s="43"/>
+    </row>
+    <row r="51" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="5"/>
       <c r="E51" s="36"/>
       <c r="F51" s="23"/>
-      <c r="G51" s="38"/>
-      <c r="H51" s="39"/>
-      <c r="I51" s="40"/>
-    </row>
-    <row r="52" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G51" s="41"/>
+      <c r="H51" s="42"/>
+      <c r="I51" s="43"/>
+    </row>
+    <row r="52" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="5"/>
       <c r="E52" s="36"/>
       <c r="F52" s="23"/>
-      <c r="G52" s="38"/>
-      <c r="H52" s="39"/>
-      <c r="I52" s="40"/>
-    </row>
-    <row r="53" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G52" s="41"/>
+      <c r="H52" s="42"/>
+      <c r="I52" s="43"/>
+    </row>
+    <row r="53" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="5"/>
       <c r="E53" s="36"/>
       <c r="F53" s="23"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="39"/>
-      <c r="I53" s="40"/>
-    </row>
-    <row r="54" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G53" s="41"/>
+      <c r="H53" s="42"/>
+      <c r="I53" s="43"/>
+    </row>
+    <row r="54" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
       <c r="E54" s="36"/>
       <c r="F54" s="23"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="39"/>
-      <c r="I54" s="40"/>
-    </row>
-    <row r="55" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G54" s="41"/>
+      <c r="H54" s="42"/>
+      <c r="I54" s="43"/>
+    </row>
+    <row r="55" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="5"/>
       <c r="E55" s="36"/>
       <c r="F55" s="23"/>
-      <c r="G55" s="38"/>
-      <c r="H55" s="39"/>
-      <c r="I55" s="40"/>
-    </row>
-    <row r="56" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G55" s="41"/>
+      <c r="H55" s="42"/>
+      <c r="I55" s="43"/>
+    </row>
+    <row r="56" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="5"/>
       <c r="E56" s="36"/>
       <c r="F56" s="23"/>
-      <c r="G56" s="38"/>
-      <c r="H56" s="39"/>
-      <c r="I56" s="40"/>
-    </row>
-    <row r="57" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G56" s="41"/>
+      <c r="H56" s="42"/>
+      <c r="I56" s="43"/>
+    </row>
+    <row r="57" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="5"/>
       <c r="E57" s="36"/>
       <c r="F57" s="23"/>
-      <c r="G57" s="38"/>
-      <c r="H57" s="39"/>
-      <c r="I57" s="40"/>
-    </row>
-    <row r="58" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G57" s="41"/>
+      <c r="H57" s="42"/>
+      <c r="I57" s="43"/>
+    </row>
+    <row r="58" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="5"/>
       <c r="E58" s="36"/>
       <c r="F58" s="23"/>
-      <c r="G58" s="38"/>
-      <c r="H58" s="39"/>
-      <c r="I58" s="40"/>
-    </row>
-    <row r="59" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G58" s="41"/>
+      <c r="H58" s="42"/>
+      <c r="I58" s="43"/>
+    </row>
+    <row r="59" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="5"/>
       <c r="E59" s="36"/>
       <c r="F59" s="23"/>
-      <c r="G59" s="38"/>
-      <c r="H59" s="39"/>
-      <c r="I59" s="40"/>
-    </row>
-    <row r="60" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G59" s="41"/>
+      <c r="H59" s="42"/>
+      <c r="I59" s="43"/>
+    </row>
+    <row r="60" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="5"/>
       <c r="E60" s="36"/>
       <c r="F60" s="23"/>
-      <c r="G60" s="38"/>
-      <c r="H60" s="39"/>
-      <c r="I60" s="40"/>
-    </row>
-    <row r="61" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G60" s="41"/>
+      <c r="H60" s="42"/>
+      <c r="I60" s="43"/>
+    </row>
+    <row r="61" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="5"/>
       <c r="E61" s="36"/>
       <c r="F61" s="23"/>
-      <c r="G61" s="38"/>
-      <c r="H61" s="39"/>
-      <c r="I61" s="40"/>
-    </row>
-    <row r="62" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G61" s="41"/>
+      <c r="H61" s="42"/>
+      <c r="I61" s="43"/>
+    </row>
+    <row r="62" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="5"/>
       <c r="E62" s="36"/>
       <c r="F62" s="23"/>
-      <c r="G62" s="38"/>
-      <c r="H62" s="39"/>
-      <c r="I62" s="40"/>
-    </row>
-    <row r="63" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G62" s="41"/>
+      <c r="H62" s="42"/>
+      <c r="I62" s="43"/>
+    </row>
+    <row r="63" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="5"/>
       <c r="E63" s="36"/>
       <c r="F63" s="23"/>
-      <c r="G63" s="38"/>
-      <c r="H63" s="39"/>
-      <c r="I63" s="40"/>
-    </row>
-    <row r="64" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G63" s="41"/>
+      <c r="H63" s="42"/>
+      <c r="I63" s="43"/>
+    </row>
+    <row r="64" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="5"/>
       <c r="E64" s="36"/>
       <c r="F64" s="23"/>
-      <c r="G64" s="38"/>
-      <c r="H64" s="39"/>
-      <c r="I64" s="40"/>
-    </row>
-    <row r="65" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G64" s="41"/>
+      <c r="H64" s="42"/>
+      <c r="I64" s="43"/>
+    </row>
+    <row r="65" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="5"/>
       <c r="E65" s="36"/>
       <c r="F65" s="23"/>
-      <c r="G65" s="38"/>
-      <c r="H65" s="39"/>
-      <c r="I65" s="40"/>
-    </row>
-    <row r="66" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G65" s="41"/>
+      <c r="H65" s="42"/>
+      <c r="I65" s="43"/>
+    </row>
+    <row r="66" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="5"/>
       <c r="E66" s="36"/>
       <c r="F66" s="23"/>
-      <c r="G66" s="38"/>
-      <c r="H66" s="39"/>
-      <c r="I66" s="40"/>
-    </row>
-    <row r="67" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G66" s="41"/>
+      <c r="H66" s="42"/>
+      <c r="I66" s="43"/>
+    </row>
+    <row r="67" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="5"/>
       <c r="E67" s="36"/>
       <c r="F67" s="23"/>
-      <c r="G67" s="38"/>
-      <c r="H67" s="39"/>
-      <c r="I67" s="40"/>
-    </row>
-    <row r="68" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G67" s="41"/>
+      <c r="H67" s="42"/>
+      <c r="I67" s="43"/>
+    </row>
+    <row r="68" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="5"/>
       <c r="E68" s="36"/>
       <c r="F68" s="23"/>
-      <c r="G68" s="38"/>
-      <c r="H68" s="39"/>
-      <c r="I68" s="40"/>
-    </row>
-    <row r="69" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G68" s="41"/>
+      <c r="H68" s="42"/>
+      <c r="I68" s="43"/>
+    </row>
+    <row r="69" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="5"/>
       <c r="E69" s="36"/>
       <c r="F69" s="23"/>
-      <c r="G69" s="38"/>
-      <c r="H69" s="39"/>
-      <c r="I69" s="40"/>
-    </row>
-    <row r="70" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G69" s="41"/>
+      <c r="H69" s="42"/>
+      <c r="I69" s="43"/>
+    </row>
+    <row r="70" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="5"/>
       <c r="E70" s="36"/>
       <c r="F70" s="23"/>
-      <c r="G70" s="38"/>
-      <c r="H70" s="39"/>
-      <c r="I70" s="40"/>
-    </row>
-    <row r="71" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G70" s="41"/>
+      <c r="H70" s="42"/>
+      <c r="I70" s="43"/>
+    </row>
+    <row r="71" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="5"/>
       <c r="E71" s="36"/>
       <c r="F71" s="23"/>
-      <c r="G71" s="38"/>
-      <c r="H71" s="39"/>
-      <c r="I71" s="40"/>
-    </row>
-    <row r="72" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G71" s="41"/>
+      <c r="H71" s="42"/>
+      <c r="I71" s="43"/>
+    </row>
+    <row r="72" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="5"/>
       <c r="E72" s="36"/>
       <c r="F72" s="23"/>
-      <c r="G72" s="38"/>
-      <c r="H72" s="39"/>
-      <c r="I72" s="40"/>
-    </row>
-    <row r="73" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G72" s="41"/>
+      <c r="H72" s="42"/>
+      <c r="I72" s="43"/>
+    </row>
+    <row r="73" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="5"/>
       <c r="E73" s="36"/>
       <c r="F73" s="23"/>
-      <c r="G73" s="38"/>
-      <c r="H73" s="39"/>
-      <c r="I73" s="40"/>
-    </row>
-    <row r="74" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G73" s="41"/>
+      <c r="H73" s="42"/>
+      <c r="I73" s="43"/>
+    </row>
+    <row r="74" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="5"/>
       <c r="E74" s="36"/>
       <c r="F74" s="23"/>
-      <c r="G74" s="38"/>
-      <c r="H74" s="39"/>
-      <c r="I74" s="40"/>
-    </row>
-    <row r="75" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G74" s="41"/>
+      <c r="H74" s="42"/>
+      <c r="I74" s="43"/>
+    </row>
+    <row r="75" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="5"/>
       <c r="E75" s="36"/>
       <c r="F75" s="23"/>
-      <c r="G75" s="38"/>
-      <c r="H75" s="39"/>
-      <c r="I75" s="40"/>
-    </row>
-    <row r="76" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G75" s="41"/>
+      <c r="H75" s="42"/>
+      <c r="I75" s="43"/>
+    </row>
+    <row r="76" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="5"/>
       <c r="E76" s="36"/>
       <c r="F76" s="23"/>
-      <c r="G76" s="38"/>
-      <c r="H76" s="39"/>
-      <c r="I76" s="40"/>
-    </row>
-    <row r="77" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G76" s="41"/>
+      <c r="H76" s="42"/>
+      <c r="I76" s="43"/>
+    </row>
+    <row r="77" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="5"/>
       <c r="E77" s="36"/>
       <c r="F77" s="23"/>
-      <c r="G77" s="38"/>
-      <c r="H77" s="39"/>
-      <c r="I77" s="40"/>
-    </row>
-    <row r="78" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G77" s="41"/>
+      <c r="H77" s="42"/>
+      <c r="I77" s="43"/>
+    </row>
+    <row r="78" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="5"/>
       <c r="E78" s="36"/>
       <c r="F78" s="23"/>
-      <c r="G78" s="38"/>
-      <c r="H78" s="39"/>
-      <c r="I78" s="40"/>
-    </row>
-    <row r="79" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G78" s="41"/>
+      <c r="H78" s="42"/>
+      <c r="I78" s="43"/>
+    </row>
+    <row r="79" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="5"/>
       <c r="E79" s="36"/>
       <c r="F79" s="23"/>
-      <c r="G79" s="38"/>
-      <c r="H79" s="39"/>
-      <c r="I79" s="40"/>
-    </row>
-    <row r="80" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G79" s="41"/>
+      <c r="H79" s="42"/>
+      <c r="I79" s="43"/>
+    </row>
+    <row r="80" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="5"/>
       <c r="E80" s="36"/>
       <c r="F80" s="23"/>
-      <c r="G80" s="38"/>
-      <c r="H80" s="39"/>
-      <c r="I80" s="40"/>
-    </row>
-    <row r="81" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G80" s="41"/>
+      <c r="H80" s="42"/>
+      <c r="I80" s="43"/>
+    </row>
+    <row r="81" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
       <c r="D81" s="5"/>
       <c r="E81" s="36"/>
       <c r="F81" s="23"/>
-      <c r="G81" s="38"/>
-      <c r="H81" s="39"/>
-      <c r="I81" s="40"/>
-    </row>
-    <row r="82" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G81" s="41"/>
+      <c r="H81" s="42"/>
+      <c r="I81" s="43"/>
+    </row>
+    <row r="82" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="5"/>
       <c r="E82" s="36"/>
       <c r="F82" s="23"/>
-      <c r="G82" s="38"/>
-      <c r="H82" s="39"/>
-      <c r="I82" s="40"/>
-    </row>
-    <row r="83" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G82" s="41"/>
+      <c r="H82" s="42"/>
+      <c r="I82" s="43"/>
+    </row>
+    <row r="83" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="5"/>
       <c r="E83" s="36"/>
       <c r="F83" s="23"/>
-      <c r="G83" s="38"/>
-      <c r="H83" s="39"/>
-      <c r="I83" s="40"/>
-    </row>
-    <row r="84" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G83" s="41"/>
+      <c r="H83" s="42"/>
+      <c r="I83" s="43"/>
+    </row>
+    <row r="84" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="5"/>
       <c r="E84" s="36"/>
       <c r="F84" s="23"/>
-      <c r="G84" s="38"/>
-      <c r="H84" s="39"/>
-      <c r="I84" s="40"/>
-    </row>
-    <row r="85" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G84" s="41"/>
+      <c r="H84" s="42"/>
+      <c r="I84" s="43"/>
+    </row>
+    <row r="85" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="5"/>
       <c r="E85" s="36"/>
       <c r="F85" s="23"/>
-      <c r="G85" s="38"/>
-      <c r="H85" s="39"/>
-      <c r="I85" s="40"/>
-    </row>
-    <row r="86" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G85" s="41"/>
+      <c r="H85" s="42"/>
+      <c r="I85" s="43"/>
+    </row>
+    <row r="86" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="5"/>
       <c r="E86" s="36"/>
       <c r="F86" s="23"/>
-      <c r="G86" s="38"/>
-      <c r="H86" s="39"/>
-      <c r="I86" s="40"/>
-    </row>
-    <row r="87" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G86" s="41"/>
+      <c r="H86" s="42"/>
+      <c r="I86" s="43"/>
+    </row>
+    <row r="87" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="5"/>
       <c r="E87" s="36"/>
       <c r="F87" s="23"/>
-      <c r="G87" s="38"/>
-      <c r="H87" s="39"/>
-      <c r="I87" s="40"/>
-    </row>
-    <row r="88" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G87" s="41"/>
+      <c r="H87" s="42"/>
+      <c r="I87" s="43"/>
+    </row>
+    <row r="88" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="5"/>
       <c r="E88" s="36"/>
       <c r="F88" s="23"/>
-      <c r="G88" s="38"/>
-      <c r="H88" s="39"/>
-      <c r="I88" s="40"/>
-    </row>
-    <row r="89" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G88" s="41"/>
+      <c r="H88" s="42"/>
+      <c r="I88" s="43"/>
+    </row>
+    <row r="89" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="5"/>
       <c r="E89" s="36"/>
       <c r="F89" s="23"/>
-      <c r="G89" s="38"/>
-      <c r="H89" s="39"/>
-      <c r="I89" s="40"/>
-    </row>
-    <row r="90" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G89" s="41"/>
+      <c r="H89" s="42"/>
+      <c r="I89" s="43"/>
+    </row>
+    <row r="90" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="5"/>
       <c r="E90" s="36"/>
       <c r="F90" s="23"/>
-      <c r="G90" s="38"/>
-      <c r="H90" s="39"/>
-      <c r="I90" s="40"/>
-    </row>
-    <row r="91" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G90" s="41"/>
+      <c r="H90" s="42"/>
+      <c r="I90" s="43"/>
+    </row>
+    <row r="91" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="5"/>
       <c r="E91" s="36"/>
       <c r="F91" s="23"/>
-      <c r="G91" s="38"/>
-      <c r="H91" s="39"/>
-      <c r="I91" s="40"/>
-    </row>
-    <row r="92" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G91" s="41"/>
+      <c r="H91" s="42"/>
+      <c r="I91" s="43"/>
+    </row>
+    <row r="92" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="5"/>
       <c r="E92" s="36"/>
       <c r="F92" s="23"/>
-      <c r="G92" s="38"/>
-      <c r="H92" s="39"/>
-      <c r="I92" s="40"/>
-    </row>
-    <row r="93" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G92" s="41"/>
+      <c r="H92" s="42"/>
+      <c r="I92" s="43"/>
+    </row>
+    <row r="93" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="5"/>
       <c r="E93" s="36"/>
       <c r="F93" s="23"/>
-      <c r="G93" s="38"/>
-      <c r="H93" s="39"/>
-      <c r="I93" s="40"/>
-    </row>
-    <row r="94" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G93" s="41"/>
+      <c r="H93" s="42"/>
+      <c r="I93" s="43"/>
+    </row>
+    <row r="94" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="5"/>
       <c r="E94" s="36"/>
       <c r="F94" s="23"/>
-      <c r="G94" s="38"/>
-      <c r="H94" s="39"/>
-      <c r="I94" s="40"/>
-    </row>
-    <row r="95" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G94" s="41"/>
+      <c r="H94" s="42"/>
+      <c r="I94" s="43"/>
+    </row>
+    <row r="95" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="5"/>
       <c r="E95" s="36"/>
       <c r="F95" s="23"/>
-      <c r="G95" s="38"/>
-      <c r="H95" s="39"/>
-      <c r="I95" s="40"/>
-    </row>
-    <row r="96" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G95" s="41"/>
+      <c r="H95" s="42"/>
+      <c r="I95" s="43"/>
+    </row>
+    <row r="96" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="5"/>
       <c r="E96" s="36"/>
       <c r="F96" s="23"/>
-      <c r="G96" s="38"/>
-      <c r="H96" s="39"/>
-      <c r="I96" s="40"/>
-    </row>
-    <row r="97" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G96" s="41"/>
+      <c r="H96" s="42"/>
+      <c r="I96" s="43"/>
+    </row>
+    <row r="97" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="5"/>
       <c r="E97" s="36"/>
       <c r="F97" s="23"/>
-      <c r="G97" s="38"/>
-      <c r="H97" s="39"/>
-      <c r="I97" s="40"/>
-    </row>
-    <row r="98" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G97" s="41"/>
+      <c r="H97" s="42"/>
+      <c r="I97" s="43"/>
+    </row>
+    <row r="98" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="5"/>
       <c r="E98" s="36"/>
       <c r="F98" s="23"/>
-      <c r="G98" s="38"/>
-      <c r="H98" s="39"/>
-      <c r="I98" s="40"/>
-    </row>
-    <row r="99" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G98" s="41"/>
+      <c r="H98" s="42"/>
+      <c r="I98" s="43"/>
+    </row>
+    <row r="99" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="5"/>
       <c r="E99" s="36"/>
       <c r="F99" s="23"/>
-      <c r="G99" s="38"/>
-      <c r="H99" s="39"/>
-      <c r="I99" s="40"/>
-    </row>
-    <row r="100" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G99" s="41"/>
+      <c r="H99" s="42"/>
+      <c r="I99" s="43"/>
+    </row>
+    <row r="100" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="5"/>
       <c r="E100" s="36"/>
       <c r="F100" s="23"/>
-      <c r="G100" s="38"/>
-      <c r="H100" s="39"/>
-      <c r="I100" s="40"/>
+      <c r="G100" s="41"/>
+      <c r="H100" s="42"/>
+      <c r="I100" s="43"/>
     </row>
     <row r="101" spans="1:9" ht="39" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="104">
+    <mergeCell ref="G96:I96"/>
+    <mergeCell ref="G97:I97"/>
+    <mergeCell ref="G98:I98"/>
+    <mergeCell ref="G99:I99"/>
+    <mergeCell ref="G100:I100"/>
+    <mergeCell ref="G91:I91"/>
+    <mergeCell ref="G92:I92"/>
+    <mergeCell ref="G93:I93"/>
+    <mergeCell ref="G94:I94"/>
+    <mergeCell ref="G95:I95"/>
+    <mergeCell ref="G86:I86"/>
+    <mergeCell ref="G87:I87"/>
+    <mergeCell ref="G88:I88"/>
+    <mergeCell ref="G89:I89"/>
+    <mergeCell ref="G90:I90"/>
+    <mergeCell ref="G81:I81"/>
+    <mergeCell ref="G82:I82"/>
+    <mergeCell ref="G83:I83"/>
+    <mergeCell ref="G84:I84"/>
+    <mergeCell ref="G85:I85"/>
+    <mergeCell ref="G76:I76"/>
+    <mergeCell ref="G77:I77"/>
+    <mergeCell ref="G78:I78"/>
+    <mergeCell ref="G79:I79"/>
+    <mergeCell ref="G80:I80"/>
+    <mergeCell ref="G71:I71"/>
+    <mergeCell ref="G72:I72"/>
+    <mergeCell ref="G73:I73"/>
+    <mergeCell ref="G74:I74"/>
+    <mergeCell ref="G75:I75"/>
+    <mergeCell ref="G66:I66"/>
+    <mergeCell ref="G67:I67"/>
+    <mergeCell ref="G68:I68"/>
+    <mergeCell ref="G69:I69"/>
+    <mergeCell ref="G70:I70"/>
+    <mergeCell ref="G61:I61"/>
+    <mergeCell ref="G62:I62"/>
+    <mergeCell ref="G63:I63"/>
+    <mergeCell ref="G64:I64"/>
+    <mergeCell ref="G65:I65"/>
+    <mergeCell ref="G56:I56"/>
+    <mergeCell ref="G57:I57"/>
+    <mergeCell ref="G58:I58"/>
+    <mergeCell ref="G59:I59"/>
+    <mergeCell ref="G60:I60"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="G52:I52"/>
+    <mergeCell ref="G53:I53"/>
+    <mergeCell ref="G54:I54"/>
+    <mergeCell ref="G55:I55"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G8:I8"/>
@@ -2704,105 +2794,10 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="C2:G2"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="G50:I50"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="G56:I56"/>
-    <mergeCell ref="G57:I57"/>
-    <mergeCell ref="G58:I58"/>
-    <mergeCell ref="G59:I59"/>
-    <mergeCell ref="G60:I60"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="G53:I53"/>
-    <mergeCell ref="G54:I54"/>
-    <mergeCell ref="G55:I55"/>
-    <mergeCell ref="G66:I66"/>
-    <mergeCell ref="G67:I67"/>
-    <mergeCell ref="G68:I68"/>
-    <mergeCell ref="G69:I69"/>
-    <mergeCell ref="G70:I70"/>
-    <mergeCell ref="G61:I61"/>
-    <mergeCell ref="G62:I62"/>
-    <mergeCell ref="G63:I63"/>
-    <mergeCell ref="G64:I64"/>
-    <mergeCell ref="G65:I65"/>
-    <mergeCell ref="G76:I76"/>
-    <mergeCell ref="G77:I77"/>
-    <mergeCell ref="G78:I78"/>
-    <mergeCell ref="G79:I79"/>
-    <mergeCell ref="G80:I80"/>
-    <mergeCell ref="G71:I71"/>
-    <mergeCell ref="G72:I72"/>
-    <mergeCell ref="G73:I73"/>
-    <mergeCell ref="G74:I74"/>
-    <mergeCell ref="G75:I75"/>
-    <mergeCell ref="G86:I86"/>
-    <mergeCell ref="G87:I87"/>
-    <mergeCell ref="G88:I88"/>
-    <mergeCell ref="G89:I89"/>
-    <mergeCell ref="G90:I90"/>
-    <mergeCell ref="G81:I81"/>
-    <mergeCell ref="G82:I82"/>
-    <mergeCell ref="G83:I83"/>
-    <mergeCell ref="G84:I84"/>
-    <mergeCell ref="G85:I85"/>
-    <mergeCell ref="G96:I96"/>
-    <mergeCell ref="G97:I97"/>
-    <mergeCell ref="G98:I98"/>
-    <mergeCell ref="G99:I99"/>
-    <mergeCell ref="G100:I100"/>
-    <mergeCell ref="G91:I91"/>
-    <mergeCell ref="G92:I92"/>
-    <mergeCell ref="G93:I93"/>
-    <mergeCell ref="G94:I94"/>
-    <mergeCell ref="G95:I95"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.47222222222222221" right="0.56944444444444442" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2814,9 +2809,9 @@
       <selection activeCell="B4" sqref="B4:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.875" style="17" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" style="17" customWidth="1"/>
     <col min="2" max="4" width="15" style="17" customWidth="1"/>
     <col min="5" max="5" width="16.5" style="17" customWidth="1"/>
     <col min="6" max="16384" width="15" style="17" hidden="1"/>
@@ -2844,7 +2839,7 @@
       <c r="D2" s="62"/>
       <c r="E2" s="63"/>
     </row>
-    <row r="3" spans="1:5" ht="135.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="136" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>18</v>
       </c>
@@ -2853,7 +2848,7 @@
       <c r="D3" s="64"/>
       <c r="E3" s="65"/>
     </row>
-    <row r="4" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="46" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>28</v>
       </c>
@@ -2862,7 +2857,7 @@
       <c r="D4" s="69"/>
       <c r="E4" s="70"/>
     </row>
-    <row r="5" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="46" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>19</v>
       </c>
@@ -2873,7 +2868,7 @@
       <c r="D5" s="64"/>
       <c r="E5" s="65"/>
     </row>
-    <row r="6" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="46" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>17</v>
       </c>
@@ -2882,7 +2877,7 @@
       <c r="D6" s="64"/>
       <c r="E6" s="65"/>
     </row>
-    <row r="7" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="46" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>31</v>
       </c>
@@ -2914,11 +2909,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2926,16 +2916,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageLayout" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.125" style="2" customWidth="1"/>
-    <col min="2" max="6" width="10.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="2" hidden="1"/>
+    <col min="1" max="1" width="14.1640625" style="2" customWidth="1"/>
+    <col min="2" max="6" width="10.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -2973,7 +2963,7 @@
       <c r="F3" s="64"/>
       <c r="G3" s="65"/>
     </row>
-    <row r="4" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="112" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>6</v>
       </c>
@@ -3011,12 +3001,12 @@
       <c r="A8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="79"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="75"/>
     </row>
     <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
@@ -3029,7 +3019,7 @@
       <c r="F9" s="64"/>
       <c r="G9" s="65"/>
     </row>
-    <row r="10" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="112" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>6</v>
       </c>
@@ -3044,12 +3034,12 @@
       <c r="A11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="81"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="77"/>
     </row>
     <row r="12" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3068,12 +3058,12 @@
       <c r="A15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="75"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="79"/>
     </row>
     <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
@@ -3086,7 +3076,7 @@
       <c r="F16" s="64"/>
       <c r="G16" s="65"/>
     </row>
-    <row r="17" spans="1:7" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="113" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
         <v>6</v>
       </c>
@@ -3097,45 +3087,40 @@
       <c r="F17" s="64"/>
       <c r="G17" s="65"/>
     </row>
-    <row r="18" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="77"/>
-    </row>
-    <row r="19" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B18" s="80"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="81"/>
+    </row>
+    <row r="19" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3145,13 +3130,8 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>